<commit_message>
update to Hec.Dss 1.2
more unit tests
</commit_message>
<xml_diff>
--- a/test-files/small-ir-ts.xlsx
+++ b/test-files/small-ir-ts.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DSSExcelPlugin\DSSExcelTests\test-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\DSSExcel\test-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0531F5CD-7B4D-47C7-9D9E-D03F3062FF0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A536D67-258E-460C-8C35-E44EC3D3E93D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="405" windowWidth="15330" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6460" yWindow="690" windowWidth="18240" windowHeight="10400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>A</t>
   </si>
@@ -67,15 +76,6 @@
   </si>
   <si>
     <t>INST-VAL</t>
-  </si>
-  <si>
-    <t>Index</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -402,20 +402,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,7 +426,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -437,7 +437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -448,7 +448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -459,7 +459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -470,7 +470,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -481,7 +481,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -492,125 +492,124 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>43982.958333333336</v>
+      </c>
+      <c r="C8" s="3">
+        <f>-1</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2">
-        <v>43982.958333333336</v>
+        <v>43982.96875</v>
       </c>
       <c r="C9" s="3">
+        <f>C8+1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2">
+        <v>43982.979166666664</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" ref="C10:C17" si="0">C9+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2">
+        <v>43982.989583333336</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="B10" s="2">
-        <v>43982.96875</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2">
+        <v>43983</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B11" s="2">
-        <v>43982.979166666664</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2">
+        <v>43983.010416666664</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B12" s="2">
-        <v>43982.989583333336</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2">
+        <v>43983.020833333336</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B13" s="2">
-        <v>43983</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2">
+        <v>43983.03125</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B14" s="2">
-        <v>43983.010416666664</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2">
+        <v>43983.041666666664</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B15" s="2">
-        <v>43983.020833333336</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2">
+        <v>43983.197916666664</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="0"/>
         <v>8</v>
-      </c>
-      <c r="B16" s="2">
-        <v>43983.03125</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>9</v>
-      </c>
-      <c r="B17" s="2">
-        <v>43983.041666666664</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>10</v>
-      </c>
-      <c r="B18" s="2">
-        <v>43983.197916666664</v>
-      </c>
-      <c r="C18" s="3">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>